<commit_message>
Gli algoritmi vengono ripetuti fino a quando l'esecuzione non ci impiega 1 sec
</commit_message>
<xml_diff>
--- a/second assignment/result.xlsx
+++ b/second assignment/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davide/Sviluppo/Advanced Algorithm/second assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C579826-600A-2949-9B35-8E11D45DFD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AFD305-CBEA-F445-83A6-EFA6B94CA3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="760" windowWidth="29140" windowHeight="18880" xr2:uid="{C8CDD62A-8590-BD4B-8D49-6903D2629F1C}"/>
+    <workbookView xWindow="-1240" yWindow="-15500" windowWidth="29140" windowHeight="18880" xr2:uid="{C8CDD62A-8590-BD4B-8D49-6903D2629F1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Instance</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Solution</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
@@ -98,6 +95,12 @@
   </si>
   <si>
     <t>Closest Insertion</t>
+  </si>
+  <si>
+    <t>N Execution</t>
+  </si>
+  <si>
+    <t>Time(ms)</t>
   </si>
 </sst>
 </file>
@@ -191,7 +194,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -201,6 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -515,590 +518,722 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FD008E-1479-1149-A6C0-2F37AA540936}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="6"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>49336</v>
+        <v>8980</v>
       </c>
       <c r="C3">
-        <v>14.544</v>
+        <v>0.42599999999999999</v>
       </c>
       <c r="D3">
-        <f>(B3-$K3)/$K3</f>
-        <v>0.22848605577689243</v>
-      </c>
-      <c r="E3" s="3">
-        <v>47170</v>
+        <v>2348</v>
+      </c>
+      <c r="E3">
+        <f>(B3-$N3)/$N3</f>
+        <v>0.19066560594006896</v>
       </c>
       <c r="F3" s="3">
-        <v>286.298</v>
+        <v>8991</v>
       </c>
       <c r="G3">
-        <f>(E3-$K3)/$K3</f>
-        <v>0.17455179282868527</v>
+        <v>5.1040000000000001</v>
       </c>
       <c r="H3">
-        <v>51990</v>
+        <v>196</v>
       </c>
       <c r="I3">
-        <v>14.795</v>
+        <f>(F3-$N3)/$N3</f>
+        <v>0.19212410501193317</v>
       </c>
       <c r="J3">
-        <f>(H3-$K3)/$K3</f>
-        <v>0.29457171314741037</v>
+        <v>10114</v>
       </c>
       <c r="K3">
-        <v>40160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="L3">
+        <v>2033</v>
+      </c>
+      <c r="M3">
+        <f>(J3-$N3)/$N3</f>
+        <v>0.34102360116679925</v>
+      </c>
+      <c r="N3">
+        <v>7542</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8980</v>
+        <v>4048</v>
       </c>
       <c r="C4">
-        <v>0.95199999999999996</v>
+        <v>0.03</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D15" si="0">(B4-$K4)/$K4</f>
-        <v>0.19066560594006896</v>
-      </c>
-      <c r="E4" s="3">
-        <v>8991</v>
+        <v>32865</v>
+      </c>
+      <c r="E4">
+        <f>(B4-$N4)/$N4</f>
+        <v>0.21817634667469155</v>
       </c>
       <c r="F4" s="3">
-        <v>5.3220000000000001</v>
+        <v>3588</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G15" si="1">(E4-$K4)/$K4</f>
-        <v>0.19212410501193317</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="H4">
-        <v>10114</v>
+        <v>6760</v>
       </c>
       <c r="I4">
-        <v>0.96799999999999997</v>
+        <f>(F4-$N4)/$N4</f>
+        <v>7.974721637074933E-2</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J15" si="2">(H4-$K4)/$K4</f>
-        <v>0.34102360116679925</v>
+        <v>3814</v>
       </c>
       <c r="K4">
-        <v>7542</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="L4">
+        <v>26912</v>
+      </c>
+      <c r="M4">
+        <f>(J4-$N4)/$N4</f>
+        <v>0.14775804995486005</v>
+      </c>
+      <c r="N4">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>4048</v>
+        <v>8191</v>
       </c>
       <c r="C5">
-        <v>3.9E-2</v>
+        <v>3.6469999999999998</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>0.21817634667469155</v>
-      </c>
-      <c r="E5" s="3">
-        <v>3588</v>
+        <v>275</v>
+      </c>
+      <c r="E5">
+        <f>(B5-$N5)/$N5</f>
+        <v>0.25474877450980393</v>
       </c>
       <c r="F5" s="3">
-        <v>0.2</v>
+        <v>7968</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
-        <v>7.974721637074933E-2</v>
+        <v>115.24</v>
       </c>
       <c r="H5">
-        <v>3814</v>
+        <v>9</v>
       </c>
       <c r="I5">
-        <v>5.7000000000000002E-2</v>
+        <f>(F5-$N5)/$N5</f>
+        <v>0.22058823529411764</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
-        <v>0.14775804995486005</v>
+        <v>8413</v>
       </c>
       <c r="K5">
-        <v>3323</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>4.194</v>
+      </c>
+      <c r="L5">
+        <v>239</v>
+      </c>
+      <c r="M5">
+        <f>(J5-$N5)/$N5</f>
+        <v>0.28875612745098039</v>
+      </c>
+      <c r="N5">
+        <v>6528</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>8191</v>
+        <v>41660</v>
       </c>
       <c r="C6">
-        <v>8.1959999999999997</v>
+        <v>43.027999999999999</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>0.25474877450980393</v>
-      </c>
-      <c r="E6" s="3">
-        <v>7968</v>
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <f>(B6-$N6)/$N6</f>
+        <v>0.19021770184560882</v>
       </c>
       <c r="F6" s="3">
-        <v>119.268</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="1"/>
-        <v>0.22058823529411764</v>
+        <v>41459</v>
+      </c>
+      <c r="G6" s="7">
+        <v>4010.3139999999999</v>
       </c>
       <c r="H6">
-        <v>8413</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>11.590999999999999</v>
+        <f>(F6-$N6)/$N6</f>
+        <v>0.18447517284726586</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
-        <v>0.28875612745098039</v>
+        <v>44953</v>
       </c>
       <c r="K6">
-        <v>6528</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>48.731999999999999</v>
+      </c>
+      <c r="L6">
+        <v>21</v>
+      </c>
+      <c r="M6">
+        <f>(J6-$N6)/$N6</f>
+        <v>0.28429804011199361</v>
+      </c>
+      <c r="N6">
+        <v>35002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>41660</v>
+        <v>24630960</v>
       </c>
       <c r="C7">
-        <v>46.723999999999997</v>
+        <v>266.32100000000003</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0.19021770184560882</v>
-      </c>
-      <c r="E7" s="3">
-        <v>41459</v>
-      </c>
-      <c r="F7" s="4">
-        <v>4186.1570000000002</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
-        <v>0.18447517284726586</v>
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <f>(B7-$N7)/$N7</f>
+        <v>0.32000920915719488</v>
+      </c>
+      <c r="F7" s="3">
+        <v>22723503</v>
+      </c>
+      <c r="G7" s="7">
+        <v>42221.125</v>
       </c>
       <c r="H7">
-        <v>44953</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>71.691999999999993</v>
+        <f>(F7-$N7)/$N7</f>
+        <v>0.21778579577536344</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
-        <v>0.28429804011199361</v>
+        <v>25086767</v>
       </c>
       <c r="K7">
-        <v>35002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>322.97899999999998</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <f>(J7-$N7)/$N7</f>
+        <v>0.34443657364474689</v>
+      </c>
+      <c r="N7">
+        <v>18659688</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>24630960</v>
+        <v>511</v>
       </c>
       <c r="C8">
-        <v>282.44600000000003</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0.32000920915719488</v>
-      </c>
-      <c r="E8" s="3">
-        <v>22723503</v>
-      </c>
-      <c r="F8" s="4">
-        <v>44646.220999999998</v>
+        <v>2450</v>
+      </c>
+      <c r="E8">
+        <f>(B8-$N8)/$N8</f>
+        <v>0.19953051643192488</v>
+      </c>
+      <c r="F8" s="3">
+        <v>494</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
-        <v>0.21778579577536344</v>
+        <v>4.9340000000000002</v>
       </c>
       <c r="H8">
-        <v>25086767</v>
+        <v>203</v>
       </c>
       <c r="I8">
-        <v>285.149</v>
+        <f>(F8-$N8)/$N8</f>
+        <v>0.15962441314553991</v>
       </c>
       <c r="J8">
-        <f t="shared" si="2"/>
-        <v>0.34443657364474689</v>
+        <v>581</v>
       </c>
       <c r="K8">
-        <v>18659688</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="L8">
+        <v>2212</v>
+      </c>
+      <c r="M8">
+        <f>(J8-$N8)/$N8</f>
+        <v>0.36384976525821594</v>
+      </c>
+      <c r="N8">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>49336</v>
+      </c>
+      <c r="C9">
+        <v>6.65</v>
+      </c>
+      <c r="D9">
+        <v>151</v>
+      </c>
+      <c r="E9">
+        <f>(B9-$N9)/$N9</f>
+        <v>0.22848605577689243</v>
+      </c>
+      <c r="F9" s="3">
+        <v>47170</v>
+      </c>
+      <c r="G9">
+        <v>280.74400000000003</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <f>(F9-$N9)/$N9</f>
+        <v>0.17455179282868527</v>
+      </c>
+      <c r="J9">
+        <v>51990</v>
+      </c>
+      <c r="K9">
+        <v>7.5469999999999997</v>
+      </c>
+      <c r="L9">
+        <v>133</v>
+      </c>
+      <c r="M9">
+        <f>(J9-$N9)/$N9</f>
+        <v>0.29457171314741037</v>
+      </c>
+      <c r="N9">
+        <v>40160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>11</v>
-      </c>
-      <c r="B9">
-        <v>511</v>
-      </c>
-      <c r="C9">
-        <v>0.88900000000000001</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0.19953051643192488</v>
-      </c>
-      <c r="E9" s="3">
-        <v>494</v>
-      </c>
-      <c r="F9" s="3">
-        <v>5.125</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="1"/>
-        <v>0.15962441314553991</v>
-      </c>
-      <c r="H9">
-        <v>581</v>
-      </c>
-      <c r="I9">
-        <v>0.89300000000000002</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="2"/>
-        <v>0.36384976525821594</v>
-      </c>
-      <c r="K9">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
       </c>
       <c r="B10">
         <v>162430</v>
       </c>
       <c r="C10">
-        <v>19.536000000000001</v>
+        <v>8.7260000000000009</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+      <c r="E10">
+        <f>(B10-$N10)/$N10</f>
         <v>0.2067428418597049</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>156823</v>
       </c>
-      <c r="F10" s="3">
-        <v>435.07</v>
-      </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <v>421.81</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <f>(F10-$N10)/$N10</f>
         <v>0.16508670004903345</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>180152</v>
       </c>
-      <c r="I10">
-        <v>17.978999999999999</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="2"/>
+      <c r="K10">
+        <v>9.8219999999999992</v>
+      </c>
+      <c r="L10">
+        <v>102</v>
+      </c>
+      <c r="M10">
+        <f>(J10-$N10)/$N10</f>
         <v>0.33840507570467004</v>
       </c>
-      <c r="K10" s="2">
+      <c r="N10" s="2">
         <v>134602</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>27807</v>
       </c>
       <c r="C11">
-        <v>1.649</v>
+        <v>1.601</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <v>625</v>
+      </c>
+      <c r="E11">
+        <f>(B11-$N11)/$N11</f>
         <v>0.30659712433042008</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="3">
         <v>25868</v>
       </c>
-      <c r="F11" s="3">
-        <v>38.345999999999997</v>
-      </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <v>33.802</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
+      </c>
+      <c r="I11">
+        <f>(F11-$N11)/$N11</f>
         <v>0.21548726623437647</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>27210</v>
       </c>
-      <c r="I11">
-        <v>2.0129999999999999</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="2"/>
+      <c r="K11">
+        <v>1.8</v>
+      </c>
+      <c r="L11">
+        <v>556</v>
+      </c>
+      <c r="M11">
+        <f>(J11-$N11)/$N11</f>
         <v>0.27854524950662529</v>
       </c>
-      <c r="K11">
+      <c r="N11">
         <v>21282</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>26947</v>
       </c>
       <c r="C12">
-        <v>3.4260000000000002</v>
+        <v>1.589</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="E12">
+        <f>(B12-$N12)/$N12</f>
         <v>0.26547384239691935</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="3">
         <v>25219</v>
       </c>
-      <c r="F12" s="3">
-        <v>41.043999999999997</v>
-      </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <v>34.317</v>
+      </c>
+      <c r="H12">
+        <v>30</v>
+      </c>
+      <c r="I12">
+        <f>(F12-$N12)/$N12</f>
         <v>0.18432422278576124</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>27112</v>
       </c>
-      <c r="I12">
-        <v>6.7169999999999996</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="2"/>
+      <c r="K12">
+        <v>1.835</v>
+      </c>
+      <c r="L12">
+        <v>545</v>
+      </c>
+      <c r="M12">
+        <f>(J12-$N12)/$N12</f>
         <v>0.27322250399173476</v>
       </c>
-      <c r="K12">
+      <c r="N12">
         <v>21294</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>61979</v>
       </c>
       <c r="C13">
-        <v>69.108999999999995</v>
+        <v>39.296999999999997</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E13">
+        <f>(B13-$N13)/$N13</f>
         <v>0.22058765607152703</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F13" s="3">
         <v>61119</v>
       </c>
-      <c r="F13" s="4">
-        <v>3277.1320000000001</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
+      <c r="G13" s="7">
+        <v>3089.46</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <f>(F13-$N13)/$N13</f>
         <v>0.20365118752215527</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>69623</v>
       </c>
-      <c r="I13">
-        <v>68.078999999999994</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="2"/>
+      <c r="K13">
+        <v>43.673999999999999</v>
+      </c>
+      <c r="L13">
+        <v>23</v>
+      </c>
+      <c r="M13">
+        <f>(J13-$N13)/$N13</f>
         <v>0.37112529048012921</v>
       </c>
-      <c r="K13">
+      <c r="N13">
         <v>50778</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>9988</v>
       </c>
       <c r="C14">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <v>25148</v>
+      </c>
+      <c r="E14">
+        <f>(B14-$N14)/$N14</f>
         <v>0.45618894882635952</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="3">
         <v>7712</v>
       </c>
-      <c r="F14" s="3">
-        <v>0.23899999999999999</v>
-      </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="H14">
+        <v>4716</v>
+      </c>
+      <c r="I14">
+        <f>(F14-$N14)/$N14</f>
         <v>0.12436215191718909</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>7903</v>
       </c>
-      <c r="I14">
-        <v>0.108</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="2"/>
+      <c r="K14">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="L14">
+        <v>20425</v>
+      </c>
+      <c r="M14">
+        <f>(J14-$N14)/$N14</f>
         <v>0.15220877678961947</v>
       </c>
-      <c r="K14">
+      <c r="N14">
         <v>6859</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>10586</v>
       </c>
       <c r="C15">
-        <v>8.1000000000000003E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <v>13163</v>
+      </c>
+      <c r="E15">
+        <f>(B15-$N15)/$N15</f>
         <v>0.50948238984742622</v>
       </c>
-      <c r="E15" s="3">
+      <c r="F15" s="3">
         <v>7816</v>
       </c>
-      <c r="F15" s="3">
-        <v>0.53100000000000003</v>
-      </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="H15">
+        <v>2036</v>
+      </c>
+      <c r="I15">
+        <f>(F15-$N15)/$N15</f>
         <v>0.11450163981177813</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>8401</v>
       </c>
-      <c r="I15">
-        <v>0.11</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="2"/>
+      <c r="K15">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="L15">
+        <v>11302</v>
+      </c>
+      <c r="M15">
+        <f>(J15-$N15)/$N15</f>
         <v>0.19791815200342222</v>
       </c>
-      <c r="K15">
+      <c r="N15">
         <v>7013</v>
       </c>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D17">
-        <f>AVERAGE(D3:D15)</f>
-        <v>0.27437746258988793</v>
-      </c>
-      <c r="G17">
-        <f>AVERAGE(G3:G15)</f>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <f>AVERAGE(E3:E15)</f>
+        <v>0.27437746258988782</v>
+      </c>
+      <c r="I17">
+        <f>AVERAGE(I3:I15)</f>
         <v>0.17202383843030372</v>
       </c>
-      <c r="J17">
-        <f>AVERAGE(J3:J15)</f>
-        <v>0.28277837840086217</v>
+      <c r="M17">
+        <f>AVERAGE(M3:M15)</f>
+        <v>0.28277837840086212</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:N15">
+    <sortCondition ref="A3:A15"/>
+  </sortState>
   <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>